<commit_message>
updated the system prompts, fixed parsing, and improved the heat map
</commit_message>
<xml_diff>
--- a/results/information_quality_agreements.xlsx
+++ b/results/information_quality_agreements.xlsx
@@ -509,25 +509,17 @@
           <t>Accuracy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E2" t="n">
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -581,25 +573,15 @@
           <t>Trustworthness</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -653,25 +635,11 @@
           <t>Objectivity</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -725,26 +693,10 @@
           <t>Appropriateness</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>A+</t>
@@ -797,31 +749,11 @@
           <t>Relevance</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>A+</t>
@@ -869,36 +801,12 @@
           <t>Completeness</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>A−</t>
@@ -941,41 +849,13 @@
           <t>Conciseness</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>A−</t>
@@ -1013,46 +893,14 @@
           <t>Consistency</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
           <t>A+</t>
@@ -1085,51 +933,15 @@
           <t>Underestandability</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
           <t>A+</t>
@@ -1157,56 +969,16 @@
           <t>Interpretability</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
           <t>A+</t>
@@ -1229,61 +1001,17 @@
           <t>Flexibility</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
           <t>A+</t>
@@ -1301,66 +1029,18 @@
           <t>Satisfaction</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
           <t>A+</t>
@@ -1373,71 +1053,19 @@
           <t>Use Intention</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1536,37 +1164,37 @@
         <v>100</v>
       </c>
       <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I2" t="n">
+        <v>60</v>
+      </c>
+      <c r="J2" t="n">
         <v>80</v>
       </c>
-      <c r="E2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="K2" t="n">
+        <v>100</v>
+      </c>
+      <c r="L2" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2" t="n">
         <v>80</v>
       </c>
-      <c r="G2" t="n">
+      <c r="N2" t="n">
         <v>80</v>
-      </c>
-      <c r="H2" t="n">
-        <v>100</v>
-      </c>
-      <c r="I2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J2" t="n">
-        <v>60</v>
-      </c>
-      <c r="K2" t="n">
-        <v>60</v>
-      </c>
-      <c r="L2" t="n">
-        <v>100</v>
-      </c>
-      <c r="M2" t="n">
-        <v>60</v>
-      </c>
-      <c r="N2" t="n">
-        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -1578,37 +1206,37 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
         <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="J3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L3" t="n">
         <v>100</v>
       </c>
       <c r="M3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -1624,31 +1252,31 @@
         <v>100</v>
       </c>
       <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" t="n">
+        <v>60</v>
+      </c>
+      <c r="J4" t="n">
+        <v>100</v>
+      </c>
+      <c r="K4" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" t="n">
         <v>80</v>
       </c>
-      <c r="G4" t="n">
+      <c r="N4" t="n">
         <v>80</v>
-      </c>
-      <c r="H4" t="n">
-        <v>100</v>
-      </c>
-      <c r="I4" t="n">
-        <v>100</v>
-      </c>
-      <c r="J4" t="n">
-        <v>60</v>
-      </c>
-      <c r="K4" t="n">
-        <v>60</v>
-      </c>
-      <c r="L4" t="n">
-        <v>100</v>
-      </c>
-      <c r="M4" t="n">
-        <v>60</v>
-      </c>
-      <c r="N4" t="n">
-        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1662,31 +1290,31 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="I5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="J5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -1701,28 +1329,28 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H6" t="n">
         <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="J6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -1738,25 +1366,25 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
+        <v>100</v>
+      </c>
+      <c r="I7" t="n">
+        <v>60</v>
+      </c>
+      <c r="J7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" t="n">
         <v>80</v>
       </c>
-      <c r="I7" t="n">
-        <v>100</v>
-      </c>
-      <c r="J7" t="n">
-        <v>80</v>
-      </c>
-      <c r="K7" t="n">
-        <v>80</v>
-      </c>
-      <c r="L7" t="n">
-        <v>60</v>
-      </c>
       <c r="M7" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N7" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -1773,22 +1401,22 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="J8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
@@ -1806,19 +1434,19 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K9" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L9" t="n">
         <v>100</v>
       </c>
       <c r="M9" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="N9" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10">
@@ -1837,16 +1465,16 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L10" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M10" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N10" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -1866,13 +1494,13 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M11" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N11" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -1893,10 +1521,10 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N12" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -2033,25 +1661,19 @@
           <t>Accuracy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>B+</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2060,7 +1682,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2070,7 +1692,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -2105,25 +1727,15 @@
           <t>Trustworthness</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -2177,39 +1789,25 @@
           <t>Objectivity</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>B−</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -2229,7 +1827,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -2249,39 +1847,23 @@
           <t>Appropriateness</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -2301,7 +1883,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -2321,39 +1903,19 @@
           <t>Relevance</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>B−</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -2393,39 +1955,15 @@
           <t>Completeness</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -2465,44 +2003,16 @@
           <t>Conciseness</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -2537,49 +2047,17 @@
           <t>Consistency</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -2609,54 +2087,18 @@
           <t>Underestandability</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -2681,59 +2123,19 @@
           <t>Interpretability</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -2753,64 +2155,20 @@
           <t>Flexibility</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -2825,69 +2183,21 @@
           <t>Satisfaction</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>A+</t>
         </is>
       </c>
     </row>
@@ -2897,71 +2207,19 @@
           <t>Use Intention</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3060,7 +2318,7 @@
         <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
         <v>100</v>
@@ -3117,7 +2375,7 @@
         <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="J3" t="n">
         <v>100</v>
@@ -3148,25 +2406,25 @@
         <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" t="n">
         <v>60</v>
       </c>
-      <c r="I4" t="n">
-        <v>100</v>
-      </c>
-      <c r="J4" t="n">
-        <v>80</v>
-      </c>
       <c r="K4" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="L4" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M4" t="n">
         <v>100</v>
@@ -3186,25 +2444,25 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I5" t="n">
         <v>100</v>
       </c>
       <c r="J5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M5" t="n">
         <v>100</v>
@@ -3228,19 +2486,19 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n">
         <v>100</v>
       </c>
       <c r="J6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M6" t="n">
         <v>100</v>
@@ -3262,19 +2520,19 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I7" t="n">
         <v>100</v>
       </c>
       <c r="J7" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K7" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L7" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M7" t="n">
         <v>100</v>
@@ -3300,13 +2558,13 @@
         <v>100</v>
       </c>
       <c r="J8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M8" t="n">
         <v>100</v>
@@ -3333,10 +2591,10 @@
         <v>100</v>
       </c>
       <c r="K9" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L9" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M9" t="n">
         <v>100</v>
@@ -3361,10 +2619,10 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M10" t="n">
         <v>100</v>

</xml_diff>